<commit_message>
Latest changes malaria project
</commit_message>
<xml_diff>
--- a/Malaria data 2021.xlsx
+++ b/Malaria data 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analyst\MALARIA ANALYTICS\TOTALS &amp; CORDINATES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163FF5AD-8A98-4420-9F83-5D3B7BFEDCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA149AAC-9CF8-4B52-9502-1549A5B35A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="246">
   <si>
     <t>orgunitlevel2</t>
   </si>
@@ -689,63 +689,7 @@
     <t>29 DAYS - 4YRS CT TOTAL</t>
   </si>
   <si>
-    <t>West Nile 0-28 days total</t>
-  </si>
-  <si>
-    <t>Sout Central</t>
-  </si>
-  <si>
-    <t>SUM</t>
-  </si>
-  <si>
-    <t>0-28 DAYS BY REGION</t>
-  </si>
-  <si>
-    <t>10-19 YRS BY REGION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Nile </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20 + YEARS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>29DAYS - 4YRS</t>
-  </si>
-  <si>
-    <t>5YRS- 9YRS</t>
-  </si>
-  <si>
-    <t>&lt;5YRS CASES</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRAND TOTAL &lt; 5Y YRS </t>
-  </si>
-  <si>
-    <t>PREG CASES</t>
-  </si>
-  <si>
-    <t>TOTAL CASES PER REGION</t>
   </si>
   <si>
     <t>Row Labels</t>
@@ -836,6 +780,9 @@
   </si>
   <si>
     <t> 30.6373</t>
+  </si>
+  <si>
+    <t>GRAND TOTALS</t>
   </si>
 </sst>
 </file>
@@ -13873,31 +13820,31 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="G3" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="I3" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -17875,7 +17822,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B141">
         <v>3212376</v>
@@ -17914,8 +17861,8 @@
   </sheetPr>
   <dimension ref="A1:BK217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18081,34 +18028,34 @@
         <v>199</v>
       </c>
       <c r="BB1" s="10" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="BC1" s="10" t="s">
         <v>178</v>
       </c>
       <c r="BD1" s="10" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="BE1" s="10" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="BF1" s="10" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="BG1" s="10" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="BI1" s="10" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="BJ1" s="10" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="BK1" s="10" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18936,7 +18883,7 @@
         <v>2.9251</v>
       </c>
       <c r="BK5" s="18" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21436,7 +21383,7 @@
         <v>0.53159999999999996</v>
       </c>
       <c r="BK17" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -22270,7 +22217,7 @@
         <v>0.28270000000000001</v>
       </c>
       <c r="BK21" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -23725,7 +23672,7 @@
         <v>0.68520000000000003</v>
       </c>
       <c r="BK28" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -28928,7 +28875,7 @@
         <v>0.68330000000000002</v>
       </c>
       <c r="BK53" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -29137,7 +29084,7 @@
         <v>1.6325000000000001</v>
       </c>
       <c r="BK54" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -31428,7 +31375,7 @@
         <v>0.81950000000000001</v>
       </c>
       <c r="BK65" s="18" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -32471,7 +32418,7 @@
         <v>0.1699</v>
       </c>
       <c r="BK70" s="18" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -35807,7 +35754,7 @@
         <v>2.3031000000000001</v>
       </c>
       <c r="BK86" s="18" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -36016,7 +35963,7 @@
         <v>3.0352000000000001</v>
       </c>
       <c r="BK87" s="18" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -38725,7 +38672,7 @@
         <v>0.82709999999999995</v>
       </c>
       <c r="BK100" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
     </row>
     <row r="101" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -41227,7 +41174,7 @@
         <v>0.61209999999999998</v>
       </c>
       <c r="BK112" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
     </row>
     <row r="113" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -42899,7 +42846,7 @@
         <v>0.28349999999999997</v>
       </c>
       <c r="BK120" s="18" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="121" spans="1:63" ht="12.5" x14ac:dyDescent="0.25">
@@ -51624,7 +51571,7 @@
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="5" t="s">
-        <v>178</v>
+        <v>245</v>
       </c>
       <c r="D163" s="6">
         <f>SUM(D2:D162)</f>
@@ -51787,9 +51734,7 @@
     </row>
     <row r="164" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3"/>
-      <c r="B164" s="14" t="s">
-        <v>217</v>
-      </c>
+      <c r="B164" s="14"/>
       <c r="C164" s="3"/>
       <c r="AL164">
         <f ca="1">SUMIF(A1:A162, "West Nile", F2:F162)</f>
@@ -51797,1029 +51742,246 @@
       </c>
     </row>
     <row r="165" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C165">
-        <f>SUMIF(A2:A162, "West Nile", F2:F162)</f>
-        <v>2472</v>
-      </c>
-      <c r="E165" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="H165" s="15" t="s">
-        <v>222</v>
-      </c>
+      <c r="B165" s="12"/>
+      <c r="E165" s="15"/>
+      <c r="H165" s="15"/>
     </row>
     <row r="166" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C166">
-        <v>1356</v>
-      </c>
-      <c r="E166" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="F166">
-        <f>SUMIF(A1:A162, "West NILE", O1:O162)</f>
-        <v>1114196</v>
-      </c>
-      <c r="H166" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="I166">
-        <f>SUMIF(A1:A162, "West NILE", R1:R162)</f>
-        <v>764734</v>
-      </c>
-      <c r="K166">
-        <f>SUMIF(A1:A162, "", BC1:BC162)</f>
-        <v>0</v>
-      </c>
+      <c r="B166" s="12"/>
+      <c r="E166" s="12"/>
+      <c r="H166" s="12"/>
       <c r="AY166">
         <f>SUMIF(A1:A162, "", BB1:BB162)</f>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C167">
-        <f>SUMIF(A2:A162, "Ankole", F2:F162)</f>
-        <v>380</v>
-      </c>
-      <c r="E167" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F167">
-        <f>SUMIF(A1:A162, "ACHOLI", O1:O162)</f>
-        <v>512872</v>
-      </c>
-      <c r="H167" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I167">
-        <f>SUMIF(A1:A162, "Acholi", R1:R162)</f>
-        <v>399130</v>
-      </c>
+      <c r="B167" s="12"/>
+      <c r="E167" s="12"/>
+      <c r="H167" s="12"/>
     </row>
     <row r="168" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C168">
-        <f>SUMIF(A2:A162, "Bugisu", F2:F162)</f>
-        <v>880</v>
-      </c>
-      <c r="E168" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F168">
-        <f>SUMIF(A1:A162, "ANKOLE", O1:O162)</f>
-        <v>135250</v>
-      </c>
-      <c r="H168" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I168">
-        <f>SUMIF(A1:A162, "ankole", R1:R162)</f>
-        <v>135166</v>
-      </c>
-      <c r="K168" s="15" t="s">
-        <v>226</v>
-      </c>
+      <c r="B168" s="11"/>
+      <c r="E168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="K168" s="15"/>
     </row>
     <row r="169" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C169">
-        <f>SUMIF(A2:A162, "Busoga", F2:F162)</f>
-        <v>1788</v>
-      </c>
-      <c r="E169" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F169">
-        <f>SUMIF(A1:A162, "BUGISU", O1:O162)</f>
-        <v>168888</v>
-      </c>
-      <c r="H169" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I169">
-        <f>SUMIF(A1:A162, "Bugisu", R1:R162)</f>
-        <v>109256</v>
-      </c>
-      <c r="K169" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="L169">
-        <f>SUMIF(A1:A162, "West Nile", BC1:BC162)</f>
-        <v>4234944</v>
-      </c>
+      <c r="B169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="H169" s="11"/>
+      <c r="K169" s="12"/>
     </row>
     <row r="170" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C170">
-        <f>SUMIF(A2:A162, "Bukedi", F2:F162)</f>
-        <v>708</v>
-      </c>
-      <c r="E170" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F170">
-        <f>SUMIF(A1:A162, "BUSOGA", O1:O162)</f>
-        <v>918522</v>
-      </c>
-      <c r="H170" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I170">
-        <f>SUMIF(A1:A162, "Busoga", R1:R162)</f>
-        <v>537234</v>
-      </c>
-      <c r="K170" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L170">
-        <f>SUMIF(A1:A162, "Acholi", BC1:BC162)</f>
-        <v>2292406</v>
-      </c>
+      <c r="B170" s="11"/>
+      <c r="E170" s="11"/>
+      <c r="H170" s="11"/>
+      <c r="K170" s="12"/>
     </row>
     <row r="171" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B171" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C171">
-        <f>SUMIF(A2:A162, "Bunyoro", F2:F162)</f>
-        <v>614</v>
-      </c>
-      <c r="E171" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F171">
-        <f>SUMIF(A1:A162, "BUKEDI", O1:O162)</f>
-        <v>486888</v>
-      </c>
-      <c r="H171" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I171">
-        <f>SUMIF(A1:A162, "Bukedi", R1:R162)</f>
-        <v>339746</v>
-      </c>
-      <c r="K171" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L171">
-        <f>SUMIF(A1:A162, "Ankole", BC1:BC162)</f>
-        <v>965456</v>
-      </c>
+      <c r="B171" s="11"/>
+      <c r="E171" s="11"/>
+      <c r="H171" s="11"/>
+      <c r="K171" s="12"/>
     </row>
     <row r="172" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C172">
-        <f>SUMIF(A2:A162, "Kampala", F2:F162)</f>
-        <v>2732</v>
-      </c>
-      <c r="E172" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F172">
-        <f>SUMIF(A1:A162, "BUNYORO", O1:O162)</f>
-        <v>271258</v>
-      </c>
-      <c r="H172" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I172">
-        <f>SUMIF(A1:A162, "Bunyoro", R1:R162)</f>
-        <v>169498</v>
-      </c>
-      <c r="K172" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L172">
-        <f>SUMIF(A1:A162, "Bugisu", BC1:BC162)</f>
-        <v>784898</v>
-      </c>
+      <c r="B172" s="11"/>
+      <c r="E172" s="11"/>
+      <c r="H172" s="11"/>
+      <c r="K172" s="11"/>
     </row>
     <row r="173" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C173">
-        <f>SUMIF(A2:A162, "South Central", F2:F162)</f>
-        <v>3100</v>
-      </c>
-      <c r="E173" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F173">
-        <f>SUMIF(A1:A162, "KAMPALA", O1:O162)</f>
-        <v>78526</v>
-      </c>
-      <c r="H173" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I173">
-        <f>SUMIF(A1:A162, "kampala", R1:R162)</f>
-        <v>63762</v>
-      </c>
-      <c r="K173" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="L173">
-        <f>SUMIF(A1:A162, "Busoga", BC1:BC162)</f>
-        <v>3377500</v>
-      </c>
+      <c r="B173" s="11"/>
+      <c r="E173" s="11"/>
+      <c r="H173" s="11"/>
+      <c r="K173" s="11"/>
     </row>
     <row r="174" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C174">
-        <f>SUMIF(A2:A162, "North Central", F2:F162)</f>
-        <v>1450</v>
-      </c>
-      <c r="E174" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="F174">
-        <f>SUMIF(A1:A162, "SOUTH CENTRAL", O1:O162)</f>
-        <v>254744</v>
-      </c>
-      <c r="H174" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I174">
-        <f>SUMIF(A1:A162, "South Central", R1:R162)</f>
-        <v>231878</v>
-      </c>
-      <c r="K174" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L174">
-        <f>SUMIF(A1:A162, "Bukedi", BC1:BC162)</f>
-        <v>1713418</v>
-      </c>
+      <c r="B174" s="11"/>
+      <c r="E174" s="11"/>
+      <c r="H174" s="11"/>
+      <c r="K174" s="11"/>
     </row>
     <row r="175" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C175">
-        <f>SUMIF(A2:A162, "Lango", F2:F162)</f>
-        <v>1096</v>
-      </c>
-      <c r="E175" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F175">
-        <f>SUMIF(A1:A162, "NORTH CENTRAL", O1:O162)</f>
-        <v>381140</v>
-      </c>
-      <c r="H175" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I175">
-        <f>SUMIF(A1:A162, "North central", R1:R162)</f>
-        <v>301310</v>
-      </c>
-      <c r="K175" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="L175">
-        <f>SUMIF(A1:A162, "Bunyoro", BC1:BC162)</f>
-        <v>1058768</v>
-      </c>
+      <c r="B175" s="11"/>
+      <c r="E175" s="11"/>
+      <c r="H175" s="11"/>
+      <c r="K175" s="11"/>
     </row>
     <row r="176" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C176">
-        <f>SUMIF(A2:A162, "Kigezi", F2:F162)</f>
-        <v>48</v>
-      </c>
-      <c r="E176" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F176">
-        <f>SUMIF(A1:A162, "LANGO", O1:O162)</f>
-        <v>375352</v>
-      </c>
-      <c r="H176" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I176">
-        <f>SUMIF(A1:A162, "Lango", R1:R162)</f>
-        <v>260538</v>
-      </c>
-      <c r="K176" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="L176">
-        <f>SUMIF(A1:A162, "Kampala", BC1:BC162)</f>
-        <v>458856</v>
-      </c>
+      <c r="B176" s="11"/>
+      <c r="E176" s="11"/>
+      <c r="H176" s="11"/>
+      <c r="K176" s="11"/>
     </row>
-    <row r="177" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C177">
-        <f>SUMIF(A2:A162, "Karamoja", F2:F162)</f>
-        <v>1286</v>
-      </c>
-      <c r="E177" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F177">
-        <f>SUMIF(A1:A162, "KIGEZI", O1:O162)</f>
-        <v>32968</v>
-      </c>
-      <c r="H177" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I177">
-        <f>SUMIF(A1:A162, "Kigezi", R1:R162)</f>
-        <v>29960</v>
-      </c>
-      <c r="K177" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="L177">
-        <f>SUMIF(A1:A162, "SoutH CENTRAL", BC1:BC162)</f>
-        <v>1515420</v>
-      </c>
+    <row r="177" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="11"/>
+      <c r="E177" s="11"/>
+      <c r="H177" s="11"/>
+      <c r="K177" s="11"/>
     </row>
-    <row r="178" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C178">
-        <f>SUMIF(A2:A162, "Teso", F2:F162)</f>
-        <v>976</v>
-      </c>
-      <c r="E178" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F178">
-        <f>SUMIF(A1:A162, "KARAMOJA", O1:O162)</f>
-        <v>436798</v>
-      </c>
-      <c r="H178" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I178">
-        <f>SUMIF(A1:A162, "Karamoja", R1:R162)</f>
-        <v>145216</v>
-      </c>
-      <c r="K178" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L178">
-        <f>SUMIF(A1:A162, "North central", BC1:BC162)</f>
-        <v>1930912</v>
-      </c>
+    <row r="178" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="11"/>
+      <c r="E178" s="11"/>
+      <c r="H178" s="11"/>
+      <c r="K178" s="11"/>
     </row>
-    <row r="179" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C179">
-        <f>SUMIF(A2:A162, "Tooro", F2:F162)</f>
-        <v>1464</v>
-      </c>
-      <c r="E179" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F179">
-        <f>SUMIF(A1:A162, "TESO", O1:O162)</f>
-        <v>351836</v>
-      </c>
-      <c r="H179" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I179">
-        <f>SUMIF(A1:A162, "Teso", R1:R162)</f>
-        <v>305608</v>
-      </c>
-      <c r="K179" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="L179">
-        <f>SUMIF(A1:A162, "LANGO", BC1:BC162)</f>
-        <v>1613424</v>
-      </c>
+    <row r="179" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="11"/>
+      <c r="E179" s="11"/>
+      <c r="H179" s="11"/>
+      <c r="K179" s="11"/>
     </row>
-    <row r="180" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C180">
-        <f>SUM(C165:C179)</f>
-        <v>20350</v>
-      </c>
-      <c r="E180" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F180">
-        <f>SUMIF(A1:A162, "TOORO", O1:O162)</f>
-        <v>271260</v>
-      </c>
-      <c r="H180" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I180">
-        <f>SUMIF(A1:A162, "Tooro", R1:R162)</f>
-        <v>211706</v>
-      </c>
-      <c r="K180" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L180">
-        <f>SUMIF(A1:A162, "KIGEZI", BC1:BC162)</f>
-        <v>234846</v>
-      </c>
+    <row r="180" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="13"/>
+      <c r="E180" s="11"/>
+      <c r="H180" s="11"/>
+      <c r="K180" s="11"/>
     </row>
-    <row r="181" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E181" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F181">
-        <f>SUM(F166:F180)</f>
-        <v>5790498</v>
-      </c>
-      <c r="H181" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="I181">
-        <f>SUM(I166:I180)</f>
-        <v>4004742</v>
-      </c>
-      <c r="K181" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L181">
-        <f>SUMIF(A1:A162, "KARAMOJA", BC1:BC162)</f>
-        <v>1054938</v>
-      </c>
+    <row r="181" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="K181" s="11"/>
     </row>
-    <row r="182" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B182" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="E182" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="K182" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L182">
-        <f>SUMIF(A1:A162, "TESO", BC1:BC162)</f>
-        <v>1806948</v>
-      </c>
+    <row r="182" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="15"/>
+      <c r="E182" s="11"/>
+      <c r="K182" s="11"/>
     </row>
-    <row r="183" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="C183">
-        <f>SUMIF(A1:A162, "West Nile", I1:I162)</f>
-        <v>1188262</v>
-      </c>
-      <c r="E183" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="F183">
-        <f>SUMIF(A1:A162, "West Nile", L1:L162)</f>
-        <v>1165280</v>
-      </c>
-      <c r="H183" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="K183" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L183">
-        <f>SUMIF(A1:A162, "TOORO", BC1:BC162)</f>
-        <v>1451790</v>
-      </c>
+    <row r="183" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="12"/>
+      <c r="E183" s="12"/>
+      <c r="H183" s="15"/>
+      <c r="K183" s="11"/>
     </row>
-    <row r="184" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B184" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C184">
-        <f>SUMIF(A1:A162, "Acholi", I1:I162)</f>
-        <v>757262</v>
-      </c>
-      <c r="E184" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F184">
-        <f>SUMIF(A1:A162, "Acholi", L1:L162)</f>
-        <v>621786</v>
-      </c>
-      <c r="H184" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="I184">
-        <f>SUMIF(A1:A162, "west Nile", BB1:BB162)</f>
-        <v>1159814</v>
-      </c>
-      <c r="K184" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="L184">
-        <f>SUM(L169:L183)</f>
-        <v>24494524</v>
-      </c>
+    <row r="184" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="12"/>
+      <c r="E184" s="12"/>
+      <c r="H184" s="12"/>
+      <c r="K184" s="13"/>
     </row>
-    <row r="185" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C185">
-        <f>SUMIF(A1:A162, "Ankole", I1:I162)</f>
-        <v>275926</v>
-      </c>
-      <c r="E185" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F185">
-        <f>SUMIF(A1:A162, "Ankole", L1:L162)</f>
-        <v>418734</v>
-      </c>
-      <c r="H185" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I185">
-        <f>SUMIF(A1:A162, "Acholi", BB1:BB162)</f>
-        <v>641632</v>
-      </c>
+    <row r="185" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B185" s="12"/>
+      <c r="E185" s="12"/>
+      <c r="H185" s="12"/>
     </row>
-    <row r="186" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C186">
-        <f>SUMIF(A1:A162, "Bugisu", I1:I162)</f>
-        <v>183074</v>
-      </c>
-      <c r="E186" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F186">
-        <f>SUMIF(A1:A162, "Bugisu", L1:L162)</f>
-        <v>322800</v>
-      </c>
-      <c r="H186" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I186">
-        <f>SUMIF(A1:A162, "Ankole", BB1:BB162)</f>
-        <v>151904</v>
-      </c>
+    <row r="186" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="11"/>
+      <c r="E186" s="11"/>
+      <c r="H186" s="12"/>
     </row>
-    <row r="187" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C187">
-        <f>SUMIF(A1:A162, "Busoga", I1:I162)</f>
-        <v>703476</v>
-      </c>
-      <c r="E187" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F187">
-        <f>SUMIF(A1:A162, "Busoga", L1:L162)</f>
-        <v>1216480</v>
-      </c>
-      <c r="H187" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I187">
-        <f>SUMIF(A1:A162, "Bugisu", BB1:BB162)</f>
-        <v>165330</v>
-      </c>
+    <row r="187" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="11"/>
+      <c r="E187" s="11"/>
+      <c r="H187" s="11"/>
     </row>
-    <row r="188" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C188">
-        <f>SUMIF(A1:A162, "Bukedi", I1:I162)</f>
-        <v>381844</v>
-      </c>
-      <c r="E188" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F188">
-        <f>SUMIF(A1:A162, "Bukedi", L1:L162)</f>
-        <v>504232</v>
-      </c>
-      <c r="H188" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I188">
-        <f>SUMIF(A1:A162, "Busoga", BB1:BB162)</f>
-        <v>969356</v>
-      </c>
+    <row r="188" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B188" s="11"/>
+      <c r="E188" s="11"/>
+      <c r="H188" s="11"/>
     </row>
-    <row r="189" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C189">
-        <f>SUMIF(A1:A162, "Bunyoro", I1:I162)</f>
-        <v>267694</v>
-      </c>
-      <c r="E189" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F189">
-        <f>SUMIF(A1:A162, "bUNYORO", L1:L162)</f>
-        <v>349704</v>
-      </c>
-      <c r="H189" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I189">
-        <f>SUMIF(A1:A162, "Bukedi", BB1:BB162)</f>
-        <v>362234</v>
-      </c>
+    <row r="189" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="11"/>
+      <c r="E189" s="11"/>
+      <c r="H189" s="11"/>
     </row>
-    <row r="190" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C190">
-        <f>SUMIF(A1:A162, "Kampala", I1:I162)</f>
-        <v>85164</v>
-      </c>
-      <c r="E190" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F190">
-        <f>SUMIF(A1:A162, "kampala", L1:L162)</f>
-        <v>228672</v>
-      </c>
-      <c r="H190" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I190">
-        <f>SUMIF(A1:A162, "Bunyoro", BB1:BB162)</f>
-        <v>299352</v>
-      </c>
+    <row r="190" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B190" s="11"/>
+      <c r="E190" s="11"/>
+      <c r="H190" s="11"/>
     </row>
-    <row r="191" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C191">
-        <f>SUMIF(A1:A162, "South Central", I1:I162)</f>
-        <v>396128</v>
-      </c>
-      <c r="E191" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="F191">
-        <f>SUMIF(A1:A162, "South Central", L1:L162)</f>
-        <v>629570</v>
-      </c>
-      <c r="H191" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I191">
-        <f>SUMIF(A1:A162, "Kampala", BB1:BB162)</f>
-        <v>97314</v>
-      </c>
+    <row r="191" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="11"/>
+      <c r="E191" s="11"/>
+      <c r="H191" s="11"/>
     </row>
-    <row r="192" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C192">
-        <f>SUMIF(A1:A162, "North Central", I1:I162)</f>
-        <v>529344</v>
-      </c>
-      <c r="E192" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F192">
-        <f>SUMIF(A1:A162, "North central", L1:L162)</f>
-        <v>717668</v>
-      </c>
-      <c r="H192" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I192">
-        <f>SUMIF(A1:A162, "South CEntral", BB1:BB162)</f>
-        <v>289446</v>
-      </c>
+    <row r="192" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="11"/>
+      <c r="E192" s="11"/>
+      <c r="H192" s="11"/>
     </row>
-    <row r="193" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C193">
-        <f>SUMIF(A1:A162, "Lango", I1:I162)</f>
-        <v>435500</v>
-      </c>
-      <c r="E193" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F193">
-        <f>SUMIF(A1:A162, "Lango", L1:L162)</f>
-        <v>540938</v>
-      </c>
-      <c r="H193" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I193">
-        <f>SUMIF(A1:A162, "noRTH CENTRAL", BB1:BB162)</f>
-        <v>473668</v>
-      </c>
+    <row r="193" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B193" s="11"/>
+      <c r="E193" s="11"/>
+      <c r="H193" s="11"/>
     </row>
-    <row r="194" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C194">
-        <f>SUMIF(A1:A162, "Kigezi", I1:I162)</f>
-        <v>70460</v>
-      </c>
-      <c r="E194" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F194">
-        <f>SUMIF(A1:A162, "Kigezi", L1:L162)</f>
-        <v>101410</v>
-      </c>
-      <c r="H194" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I194">
-        <f>SUMIF(A1:A162, "LANGO", BB1:BB162)</f>
-        <v>397270</v>
-      </c>
+    <row r="194" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="11"/>
+      <c r="E194" s="11"/>
+      <c r="H194" s="11"/>
     </row>
-    <row r="195" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C195">
-        <f>SUMIF(A1:A162, "Karamoja", I1:I162)</f>
-        <v>184870</v>
-      </c>
-      <c r="E195" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F195">
-        <f>SUMIF(A1:A162, "Karamoja", L1:L162)</f>
-        <v>286768</v>
-      </c>
-      <c r="H195" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I195">
-        <f>SUMIF(A1:A162, "KIGEZI", BB1:BB162)</f>
-        <v>36482</v>
-      </c>
+    <row r="195" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="11"/>
+      <c r="E195" s="11"/>
+      <c r="H195" s="11"/>
     </row>
-    <row r="196" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C196">
-        <f>SUMIF(A1:A162, "Teso", I1:I162)</f>
-        <v>537052</v>
-      </c>
-      <c r="E196" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F196">
-        <f>SUMIF(A1:A162, "Teso", L1:L162)</f>
-        <v>611476</v>
-      </c>
-      <c r="H196" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I196">
-        <f>SUMIF(A1:A162, "KARAMOJA", BB1:BB162)</f>
-        <v>460068</v>
-      </c>
+    <row r="196" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B196" s="11"/>
+      <c r="E196" s="11"/>
+      <c r="H196" s="11"/>
     </row>
-    <row r="197" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C197">
-        <f>SUMIF(A1:A162, "Tooro", I1:I162)</f>
-        <v>393560</v>
-      </c>
-      <c r="E197" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F197">
-        <f>SUMIF(A1:A162, "Tooro", L1:L162)</f>
-        <v>573800</v>
-      </c>
-      <c r="H197" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I197">
-        <f>SUMIF(A1:A162, "TESO", BB1:BB162)</f>
-        <v>374980</v>
-      </c>
+    <row r="197" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B197" s="11"/>
+      <c r="E197" s="11"/>
+      <c r="H197" s="11"/>
     </row>
-    <row r="198" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C198">
-        <f>SUM(C183:C197)</f>
-        <v>6389616</v>
-      </c>
-      <c r="E198" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F198">
-        <f>SUM(F183:F197)</f>
-        <v>8289318</v>
-      </c>
-      <c r="H198" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I198">
-        <f>SUMIF(A1:A162, "TOORO", BB1:BB162)</f>
-        <v>294156</v>
-      </c>
+    <row r="198" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E198" s="13"/>
+      <c r="H198" s="11"/>
     </row>
-    <row r="199" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H199" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="I199">
-        <f>SUM(I184:I198)</f>
-        <v>6173006</v>
-      </c>
+    <row r="199" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H199" s="13"/>
     </row>
-    <row r="201" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H201" s="15" t="s">
-        <v>225</v>
-      </c>
+    <row r="201" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H201" s="15"/>
     </row>
-    <row r="202" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H202" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="I202">
-        <f>SUMIF(A1:A162, "West NILE", AY1:AY162)</f>
-        <v>95326</v>
-      </c>
+    <row r="202" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H202" s="12"/>
     </row>
-    <row r="203" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H203" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I203">
-        <f>SUMIF(A1:A162, "Acholi", AY1:AY162)</f>
-        <v>51474</v>
-      </c>
+    <row r="203" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H203" s="12"/>
     </row>
-    <row r="204" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H204" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I204">
-        <f>SUMIF(A1:A162, "ankole", AY1:AY162)</f>
-        <v>11090</v>
-      </c>
+    <row r="204" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H204" s="12"/>
     </row>
-    <row r="205" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H205" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I205">
-        <f>SUMIF(A1:A162, "Bugisu", AY1:AY162)</f>
-        <v>23822</v>
-      </c>
+    <row r="205" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H205" s="11"/>
     </row>
-    <row r="206" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H206" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I206">
-        <f>SUMIF(A1:A162, "Busoga", AY1:AY162)</f>
-        <v>131384</v>
-      </c>
+    <row r="206" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H206" s="11"/>
     </row>
-    <row r="207" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H207" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I207">
-        <f>SUMIF(A1:A162, "Bukedi", AY1:AY162)</f>
-        <v>34538</v>
-      </c>
+    <row r="207" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H207" s="11"/>
     </row>
-    <row r="208" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H208" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I208">
-        <f>SUMIF(A1:A162, "Bunyoro", AY1:AY162)</f>
-        <v>42382</v>
-      </c>
+    <row r="208" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H208" s="11"/>
     </row>
-    <row r="209" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H209" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I209">
-        <f>SUMIF(A1:A162, "Kampala", AY1:AY162)</f>
-        <v>9088</v>
-      </c>
+    <row r="209" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H209" s="11"/>
     </row>
-    <row r="210" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H210" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I210">
-        <f>SUMIF(A1:A162, "South CENTRAL", AY1:AY162)</f>
-        <v>25318</v>
-      </c>
+    <row r="210" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H210" s="11"/>
     </row>
-    <row r="211" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H211" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I211">
-        <f>SUMIF(A1:A162, "North central", AY1:AY162)</f>
-        <v>52168</v>
-      </c>
+    <row r="211" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H211" s="11"/>
     </row>
-    <row r="212" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H212" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I212">
-        <f>SUMIF(A1:A162, "lango", AY1:AY162)</f>
-        <v>61098</v>
-      </c>
+    <row r="212" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H212" s="11"/>
     </row>
-    <row r="213" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H213" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I213">
-        <f>SUMIF(A1:A162, "Kigezi", AY1:AY162)</f>
-        <v>2610</v>
-      </c>
+    <row r="213" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H213" s="11"/>
     </row>
-    <row r="214" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H214" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I214">
-        <f>SUMIF(A1:A162, "karamoja", AY1:AY162)</f>
-        <v>20360</v>
-      </c>
+    <row r="214" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H214" s="11"/>
     </row>
-    <row r="215" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H215" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I215">
-        <f>SUMIF(A1:A162, "Teso", AY1:AY162)</f>
-        <v>71024</v>
-      </c>
+    <row r="215" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H215" s="11"/>
     </row>
-    <row r="216" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H216" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I216">
-        <f>SUMIF(A1:A162, "Tooro", AY1:AY162)</f>
-        <v>25724</v>
-      </c>
+    <row r="216" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H216" s="11"/>
     </row>
-    <row r="217" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H217" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="I217">
-        <f>SUM(I202:I216)</f>
-        <v>657406</v>
-      </c>
+    <row r="217" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H217" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>